<commit_message>
update rich cards for button template
</commit_message>
<xml_diff>
--- a/resources/ESI_PHA_BOT_RESP_BUILDER_EN_CA.xlsx
+++ b/resources/ESI_PHA_BOT_RESP_BUILDER_EN_CA.xlsx
@@ -5,19 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2243665\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ESI\Kore-AI-Pharmacy-Bot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977C5143-4A41-42BD-ADAE-7A2AD49DBB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2ACA5C-458F-4374-9998-B626F5E6E0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1CB3E365-0F38-41A0-882A-60B13BA55A8E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{1CB3E365-0F38-41A0-882A-60B13BA55A8E}"/>
   </bookViews>
   <sheets>
     <sheet name="PROMPTS_CONFIG" sheetId="1" r:id="rId1"/>
     <sheet name="RICH_CARDS_CONFIG" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
   <si>
     <t>RESPONSE_ID</t>
   </si>
@@ -212,6 +211,27 @@
   </si>
   <si>
     <t>I am closing our current conversation as I have not received any input from you. We can start over when you need.</t>
+  </si>
+  <si>
+    <t>ESI_PHA_WELCOME_MSG</t>
+  </si>
+  <si>
+    <t>BUTTONS</t>
+  </si>
+  <si>
+    <t>ESA_PHA_WISMO</t>
+  </si>
+  <si>
+    <t>Where is my order?</t>
+  </si>
+  <si>
+    <t>ESA_PHA_PAYMENT_BAL</t>
+  </si>
+  <si>
+    <t>Payment/Outstanding Balance</t>
+  </si>
+  <si>
+    <t>Hello, I’m Ask Iris, Express Scripts digital assistant. I'm in beta mode and still in learning phase. Here’s how I can help you right now:</t>
   </si>
 </sst>
 </file>
@@ -614,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29329887-49B3-45E3-9F81-89EC8C728205}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,6 +850,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -837,10 +868,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3A7FAE-3539-4F42-9974-BD06304157E9}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -947,6 +978,40 @@
         <v>49</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
change for button template
</commit_message>
<xml_diff>
--- a/resources/ESI_PHA_BOT_RESP_BUILDER_EN_CA.xlsx
+++ b/resources/ESI_PHA_BOT_RESP_BUILDER_EN_CA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kore-AI-Pharmacy-Bot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC2090E-5B45-485A-8F3D-8D6E096640E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB6A461-31F3-4AAE-80C5-6373C21075AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1CB3E365-0F38-41A0-882A-60B13BA55A8E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{1CB3E365-0F38-41A0-882A-60B13BA55A8E}"/>
   </bookViews>
   <sheets>
     <sheet name="PROMPTS_CONFIG" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
   <si>
     <t>RESPONSE_ID</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>Hello, I’m Ask Iris, Express Scripts digital assistant. I'm in beta mode and still in learning phase. Here’s how I can help you right now:</t>
+  </si>
+  <si>
+    <t>BUTTONS</t>
   </si>
 </sst>
 </file>
@@ -632,7 +635,7 @@
   </sheetPr>
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -867,8 +870,8 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -905,7 +908,7 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>35</v>
@@ -922,7 +925,7 @@
         <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
added code for fallback
</commit_message>
<xml_diff>
--- a/resources/ESI_PHA_BOT_RESP_BUILDER_EN_CA.xlsx
+++ b/resources/ESI_PHA_BOT_RESP_BUILDER_EN_CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kore-AI-Pharmacy-Bot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E42EA55-CEAF-4D1C-A6BC-DF59F5231DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D3CAC6-C280-4F0B-A693-B57FE711658D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1CB3E365-0F38-41A0-882A-60B13BA55A8E}"/>
   </bookViews>
@@ -70,12 +70,6 @@
     <t>ESI_PHA_ORD_INFO_ORD_ID_RESP</t>
   </si>
   <si>
-    <t>ESI_PHA_ORD_INFO_ORD_FALLBACK</t>
-  </si>
-  <si>
-    <t>We are unable to fetch the requested details at this point. Please try again after sometime.</t>
-  </si>
-  <si>
     <t>ESI_PHA_ORD_INFO_ASK_MEMBER_ID</t>
   </si>
   <si>
@@ -221,6 +215,12 @@
   </si>
   <si>
     <t>Your order for ${trxNumber} (${shippingProvider}), is ready for delivery ${shippingDate}.</t>
+  </si>
+  <si>
+    <t>We are unable to fetch the requested details at this point. Please try again after sometime.~Not sure I understood this correctly. Can you rephrase your question? ~ Sorry Please try again after sometime.</t>
+  </si>
+  <si>
+    <t>ESI_PHA_EXECUTION_FAIL_FALLBACK_MSG</t>
   </si>
 </sst>
 </file>
@@ -667,10 +667,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -703,18 +703,18 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -722,10 +722,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -733,10 +733,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
@@ -744,10 +744,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -755,10 +755,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
@@ -766,10 +766,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -777,10 +777,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -788,18 +788,18 @@
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
@@ -807,10 +807,10 @@
     </row>
     <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
@@ -818,10 +818,10 @@
     </row>
     <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
         <v>5</v>
@@ -829,10 +829,10 @@
     </row>
     <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
         <v>5</v>
@@ -840,10 +840,10 @@
     </row>
     <row r="18" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E18" t="s">
         <v>5</v>
@@ -891,126 +891,126 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="319" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>